<commit_message>
Added Issues and finished procedure log
Went through all the procedures and commented out any that are no longer used.
</commit_message>
<xml_diff>
--- a/Procedure_and_Method_log.xlsx
+++ b/Procedure_and_Method_log.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="391">
   <si>
     <t>Method Name</t>
   </si>
@@ -274,6 +274,930 @@
   </si>
   <si>
     <t>InvoiceDataUtilities</t>
+  </si>
+  <si>
+    <t>modelType</t>
+  </si>
+  <si>
+    <t>Return the Model name as a string from inputing the Model ID</t>
+  </si>
+  <si>
+    <t>brandType</t>
+  </si>
+  <si>
+    <t>Return the Brand name as a string from inputing the Brand ID</t>
+  </si>
+  <si>
+    <t>modelName</t>
+  </si>
+  <si>
+    <t>Return the Model ID as an int from inputing the Model name</t>
+  </si>
+  <si>
+    <t>Return the Brand ID as an int from inputing the Brand name</t>
+  </si>
+  <si>
+    <t>brandName</t>
+  </si>
+  <si>
+    <t>typeName</t>
+  </si>
+  <si>
+    <t>Return the Item Type as a string from inputing the the Item Type ID</t>
+  </si>
+  <si>
+    <t>insertBrand</t>
+  </si>
+  <si>
+    <t>insertModel</t>
+  </si>
+  <si>
+    <t>After inserting a new Model Name into the table the int of the new Model ID is returned</t>
+  </si>
+  <si>
+    <t>After inserting a new Brand Name into the table the int of the new Brand ID is returned</t>
+  </si>
+  <si>
+    <t>getVendorID</t>
+  </si>
+  <si>
+    <t>Return the Vendor ID as an int from inputing the Vendor name</t>
+  </si>
+  <si>
+    <t>getVendorName</t>
+  </si>
+  <si>
+    <t>Return the Vendor name as a string from inputing the Vendor ID</t>
+  </si>
+  <si>
+    <t>getClubTypeID</t>
+  </si>
+  <si>
+    <t>getClubTypeName</t>
+  </si>
+  <si>
+    <t>Returns a "typeName" (no relation to the previous typeID or typeName method) based on an int</t>
+  </si>
+  <si>
+    <t>Returns a "typeID" (no relation to the previous typeID or typeName method) based on a string</t>
+  </si>
+  <si>
+    <t>addingToCart</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Returns a Cart class item based on the object that was passed in</t>
+  </si>
+  <si>
+    <t>ConvertDBNullToString</t>
+  </si>
+  <si>
+    <t>Converts a null value to an empty string</t>
+  </si>
+  <si>
+    <t>ConvertDBNullToDouble</t>
+  </si>
+  <si>
+    <t>Converts a null value to a 0 value double</t>
+  </si>
+  <si>
+    <t>GetTaxRates</t>
+  </si>
+  <si>
+    <t>GetPSTTax</t>
+  </si>
+  <si>
+    <t>Returns GST tax rate from a now defunct table. Commenting out code.</t>
+  </si>
+  <si>
+    <t>Returns PST tax rate from a now defunct table. Commenting out code.</t>
+  </si>
+  <si>
+    <t>getItemByID</t>
+  </si>
+  <si>
+    <t>Int32, string</t>
+  </si>
+  <si>
+    <t>List&lt;Items&gt;</t>
+  </si>
+  <si>
+    <t>Returns list of items that match the Int32 that was passed in. The string is no longer used as part of this process (even though it should be).</t>
+  </si>
+  <si>
+    <t>Int32</t>
+  </si>
+  <si>
+    <t>Returns list of items that match the Int32 that was passed in. This is a duplicate of the previous method without the string input.</t>
+  </si>
+  <si>
+    <t>getquantity</t>
+  </si>
+  <si>
+    <t>removeQTYfromInventoryWithSKU</t>
+  </si>
+  <si>
+    <t>int, int, int</t>
+  </si>
+  <si>
+    <t>Returns the qty of a sku in the database based on the sku and item type</t>
+  </si>
+  <si>
+    <t>Updates the quantity of an item based on the passed in sku and item type</t>
+  </si>
+  <si>
+    <t>updateQuantity</t>
+  </si>
+  <si>
+    <t>This is an absolute duplicate procedure of the above. Should only be using one and have the other removed.</t>
+  </si>
+  <si>
+    <t>reserveTradeInSKu</t>
+  </si>
+  <si>
+    <t>Returns a SKU for a trade in based on the users location.</t>
+  </si>
+  <si>
+    <t>tradeInSku</t>
+  </si>
+  <si>
+    <t>Returns a SKU for a trade in based on the users location. Adds the SKU to a temp table.</t>
+  </si>
+  <si>
+    <t>tradeInSkuRange</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>Returns the upper and lower band ranges for a trade in sku. For the actual purposes of trade ins not sure if this is actually used as validation.</t>
+  </si>
+  <si>
+    <t>addTradeInItem</t>
+  </si>
+  <si>
+    <t>Clubs, int, int</t>
+  </si>
+  <si>
+    <t>Adds the trade in club to the trade in club table</t>
+  </si>
+  <si>
+    <t>mainInvoice</t>
+  </si>
+  <si>
+    <t>CheckoutManager, List&lt;Cart&gt;, List&lt;Checkout&gt;, Customer, Employee, int, string, string</t>
+  </si>
+  <si>
+    <t>Finalizes the invoice and saves the info to the required tables.</t>
+  </si>
+  <si>
+    <t>getNextInvoiceNum</t>
+  </si>
+  <si>
+    <t>During a new sale this will return the next invoice number in line.</t>
+  </si>
+  <si>
+    <t>createInvoiceNum</t>
+  </si>
+  <si>
+    <t>Saves the new invoice number so that another user can't use the same one.</t>
+  </si>
+  <si>
+    <t>getNextInvoiceSubNum</t>
+  </si>
+  <si>
+    <t>During an adjustment to an invoice this will return the next subnumber for the new invoice.</t>
+  </si>
+  <si>
+    <t>invoiceItem</t>
+  </si>
+  <si>
+    <t>Inserts the newly sold item into the invoice Items table</t>
+  </si>
+  <si>
+    <t>invoiceMOP</t>
+  </si>
+  <si>
+    <t>Inserts the new methods of payments into the invoice methods of payment table</t>
+  </si>
+  <si>
+    <t>returnEmployeeIDfromPassword</t>
+  </si>
+  <si>
+    <t>Returns the employee ID as an interger based on the password used.</t>
+  </si>
+  <si>
+    <t>maxSku</t>
+  </si>
+  <si>
+    <t>int, string</t>
+  </si>
+  <si>
+    <t>Returns the max sku from a table (not sure why an int of sku is being passed in).</t>
+  </si>
+  <si>
+    <t>Returns the max sku from the skunumbers table based on the itemType</t>
+  </si>
+  <si>
+    <t>storeMaxSku</t>
+  </si>
+  <si>
+    <t>Stores the max sku number into the skunumbers table</t>
+  </si>
+  <si>
+    <t>deleteInvoice</t>
+  </si>
+  <si>
+    <t>int, int, string</t>
+  </si>
+  <si>
+    <t>Deletes an invoice from the finalized tables and stores into deleted invoice table. Now that returns are working this should not need to be used at all.</t>
+  </si>
+  <si>
+    <t>getItemsToReAdd</t>
+  </si>
+  <si>
+    <t>checkInClub</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was looking in the club table to add item back in stock. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was looking in the clothing table to add item back in stock. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was looking in the accessories table to add item back in stock. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>checkInClothing</t>
+  </si>
+  <si>
+    <t>checkInAccessories</t>
+  </si>
+  <si>
+    <t>getQuantity</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was looking in the tables to return the current quantity of an item. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>reAddingItems</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was retreiving the items that are needed to add back into stock. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure was actaully adding the items back into stock. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>getInvoiceData</t>
+  </si>
+  <si>
+    <t>getInvoiceItems</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure gathers all info from tbl_invoiceItem then calls another procedure to transfer it. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure gathers all info from tbl_invoice then calls another procedure to transfer it. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>getInvoiceMOPs</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure gathers all info from tbl_invoiceMOP then calls another procedure to transfer it. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>transferMainInvoice</t>
+  </si>
+  <si>
+    <t>Invoice, string</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure adds the original data from tbl_invoice to the deleted table. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>transferInvoiceItem</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure adds the original data from tbl_invoiceItems to the deleted table. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>transferInoviceMOP</t>
+  </si>
+  <si>
+    <t>deleteInvoiceMOP</t>
+  </si>
+  <si>
+    <t>deleteInvoiceItem</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure deletes the original data from tbl_invoiceMOP. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure adds the original data from tbl_invoiceMOP to the deleted table. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>On deletion of an invoice this procedure deletes the original data from tbl_invoiceItem. Since that method is now no longer needed this one is also not needed.</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Creates an Items class item</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Creates a Location class item</t>
+  </si>
+  <si>
+    <t>LocationManager</t>
+  </si>
+  <si>
+    <t>provinceName</t>
+  </si>
+  <si>
+    <t>Returns the province name based on the province ID that was input</t>
+  </si>
+  <si>
+    <t>pronvinceID</t>
+  </si>
+  <si>
+    <t>Returns the province ID based on the province name that was input</t>
+  </si>
+  <si>
+    <t>countryName</t>
+  </si>
+  <si>
+    <t>Returns the country name based on the country ID that was input</t>
+  </si>
+  <si>
+    <t>countryID</t>
+  </si>
+  <si>
+    <t>Returns the country ID based on the country name that was input</t>
+  </si>
+  <si>
+    <t>countryIDFromProvince</t>
+  </si>
+  <si>
+    <t>Returns the country ID based on the province ID that was input</t>
+  </si>
+  <si>
+    <t>locationName</t>
+  </si>
+  <si>
+    <t>Returns the Store Name as a string based on the location ID that was input</t>
+  </si>
+  <si>
+    <t>locationID</t>
+  </si>
+  <si>
+    <t>Returns the location ID based on the Store Name that was input</t>
+  </si>
+  <si>
+    <t>locationIDfromCity</t>
+  </si>
+  <si>
+    <t>Returns the location ID based on the city name that was input</t>
+  </si>
+  <si>
+    <t>returnLocationForInvoice</t>
+  </si>
+  <si>
+    <t>Returns a Location class item based on the city name that was input</t>
+  </si>
+  <si>
+    <t>locationCity</t>
+  </si>
+  <si>
+    <t>Returns the city name based on the location ID that was input</t>
+  </si>
+  <si>
+    <t>ShowMessage</t>
+  </si>
+  <si>
+    <t>string, Page</t>
+  </si>
+  <si>
+    <t>MessageBox</t>
+  </si>
+  <si>
+    <t>Pops up a message box alert</t>
+  </si>
+  <si>
+    <t>inputBoxV2</t>
+  </si>
+  <si>
+    <t>string, string</t>
+  </si>
+  <si>
+    <t>Used for user input. Currently JavaScript is being use to replace this functionality.</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>cashoutAmounts</t>
+  </si>
+  <si>
+    <t>DateTime, DateTime, int</t>
+  </si>
+  <si>
+    <t>List&lt;Cashout&gt;</t>
+  </si>
+  <si>
+    <t>getRemainingCashout</t>
+  </si>
+  <si>
+    <t>getTradeInsCashout</t>
+  </si>
+  <si>
+    <t>Retunrs a list of Cashout that holds the MOP Type, amount, and trade in based on between 2 dates and location that was input (the trade in amount here needs to be investigated to figure out how its being used).</t>
+  </si>
+  <si>
+    <t>Returns a list of Cashout that holds the gst, pst, and subtotal for each invoice based on between 2 dates and the location that was input</t>
+  </si>
+  <si>
+    <t>Returns the amount of total trade ins based on between 2 dates and the location that was input (since this gathers the trade in amount it doesn't need top be gathered by "cashoutAmounts"</t>
+  </si>
+  <si>
+    <t>insertCashout</t>
+  </si>
+  <si>
+    <t>Saves the cashout info into the cashout table</t>
+  </si>
+  <si>
+    <t>importItems</t>
+  </si>
+  <si>
+    <t>FileUpload</t>
+  </si>
+  <si>
+    <t>Not sure if this over writes the items in all three tables or if this method just uploads new items into the three item tables.</t>
+  </si>
+  <si>
+    <t>This uploads customers, again not sure if it over writes or adds new ones. Comments mention that this doesn't work. Will need further investigation.</t>
+  </si>
+  <si>
+    <t>exportClubs</t>
+  </si>
+  <si>
+    <t>exportClothing</t>
+  </si>
+  <si>
+    <t>exportAccessories</t>
+  </si>
+  <si>
+    <t>Export clothing table to excel file in users Downloads folder</t>
+  </si>
+  <si>
+    <t>Export clubs table to excel file in users Downloads folder</t>
+  </si>
+  <si>
+    <t>Export accessories table to excel file in users Downloads folder</t>
+  </si>
+  <si>
+    <t>exportAllItems</t>
+  </si>
+  <si>
+    <t>System.Data.DataTable</t>
+  </si>
+  <si>
+    <t>Returns all items in the database in a datatable format.</t>
+  </si>
+  <si>
+    <t>exportAllAdd_Clubs</t>
+  </si>
+  <si>
+    <t>This method actually adds each row from the clubs table into the export file</t>
+  </si>
+  <si>
+    <t>exportAllAdd_Accessories</t>
+  </si>
+  <si>
+    <t>exportAllAdd_Clothing</t>
+  </si>
+  <si>
+    <t>exportAllSalesToExcel</t>
+  </si>
+  <si>
+    <t>This method actually adds each row from the accessories table into the export file</t>
+  </si>
+  <si>
+    <t>This method actually adds each row from the clothing table into the export file</t>
+  </si>
+  <si>
+    <t>Stores everything from Invoice, invoice item, and invoice mop into their own data tables</t>
+  </si>
+  <si>
+    <t>initiateInvoiceTable</t>
+  </si>
+  <si>
+    <t>Returns the columns for headers of the Invoice table then fills it and returns the info in a datatable format.</t>
+  </si>
+  <si>
+    <t>initiateInvoiceItemTable</t>
+  </si>
+  <si>
+    <t>Returns the columns for headers of the Invoice Items table then fills it and returns the info in a datatable format.</t>
+  </si>
+  <si>
+    <t>initiateInvoiceMOPTable</t>
+  </si>
+  <si>
+    <t>Returns the columns for headers of the Invoice MOP table then fills it and returns the info in a datatable format.</t>
+  </si>
+  <si>
+    <t>exportSales_Invoice</t>
+  </si>
+  <si>
+    <t>Fills the Export table line by line with all the info from the Invoice table</t>
+  </si>
+  <si>
+    <t>exportSales_Items</t>
+  </si>
+  <si>
+    <t>Fills the Export table line by line with all the info from the Invoice Items table</t>
+  </si>
+  <si>
+    <t>Fills the Export table line by line with all the info from the Invoice MOPs table</t>
+  </si>
+  <si>
+    <t>exportSales_MOP</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>SweetShopManager</t>
+  </si>
+  <si>
+    <t>GetCustomerfromSearch</t>
+  </si>
+  <si>
+    <t>List&lt;Customer&gt;</t>
+  </si>
+  <si>
+    <t>GetCustomerbyCustomerNumber</t>
+  </si>
+  <si>
+    <t>Returns a list of class Customers that match the search criteria of a string</t>
+  </si>
+  <si>
+    <t>Returns a class Customer that match the search criteria of the customer ID.</t>
+  </si>
+  <si>
+    <t>addCustomer</t>
+  </si>
+  <si>
+    <t>Adds a customer to the customer table then returns the newly created customer ID</t>
+  </si>
+  <si>
+    <t>returnCustomerNumber</t>
+  </si>
+  <si>
+    <t>Uses the information in the Customer to search the table and return the customer ID located.</t>
+  </si>
+  <si>
+    <t>updateCustomer</t>
+  </si>
+  <si>
+    <t>Updates the customer infpormation in the customer table with new info.</t>
+  </si>
+  <si>
+    <t>returnSearchFromAllThreeItemSets</t>
+  </si>
+  <si>
+    <t>Using the search string and location goes through each table to find all items that match the criteria</t>
+  </si>
+  <si>
+    <t>GetItemfromSearch</t>
+  </si>
+  <si>
+    <t>string, string, string</t>
+  </si>
+  <si>
+    <t>Looks through a table to find all items that match the search criteria. Used in returnSearchFromAllThreeItemSets.</t>
+  </si>
+  <si>
+    <t>Duplicate of the other GetItemfromSearch. This one is only used in the Inventory Home page.</t>
+  </si>
+  <si>
+    <t>tradeInItemLookUp</t>
+  </si>
+  <si>
+    <t>singleItemLookUp</t>
+  </si>
+  <si>
+    <t>Returns a Clubs class item that matched the sku that was input</t>
+  </si>
+  <si>
+    <t>Returns a Trade In club from the trade in table based on the sku that was input.</t>
+  </si>
+  <si>
+    <t>addItem</t>
+  </si>
+  <si>
+    <t>Returns the sku number of the object that was added to inventory. This calls another method to actually add the item based on what type of object was passed in.</t>
+  </si>
+  <si>
+    <t>checkForItem</t>
+  </si>
+  <si>
+    <t>Checks the object for type of item then passes to another method for processing.</t>
+  </si>
+  <si>
+    <t>returnItemNumber</t>
+  </si>
+  <si>
+    <t>Returns the sku of the object that was passed in.</t>
+  </si>
+  <si>
+    <t>addClub</t>
+  </si>
+  <si>
+    <t>Adds the club that was passed in into the clubs table.</t>
+  </si>
+  <si>
+    <t>addAccessory</t>
+  </si>
+  <si>
+    <t>Adds the accessory that was passed in into the accessories table.</t>
+  </si>
+  <si>
+    <t>addClothing</t>
+  </si>
+  <si>
+    <t>Adds the clothing that was passed in into the clothing table.</t>
+  </si>
+  <si>
+    <t>getItemType</t>
+  </si>
+  <si>
+    <t>Returns the item type (club, accessory, clothing) value based on the sku that was input</t>
+  </si>
+  <si>
+    <t>checkClubForItem</t>
+  </si>
+  <si>
+    <t>checkAccessoryForItem</t>
+  </si>
+  <si>
+    <t>checkClothingForItem</t>
+  </si>
+  <si>
+    <t>Returns bool based on the sku number that was input if the item was found in the accessories table.</t>
+  </si>
+  <si>
+    <t>Returns bool based on the sku number that was input if the item was found in the clubs table.</t>
+  </si>
+  <si>
+    <t>Returns bool based on the sku number that was input if the item was found in the clothing table.</t>
+  </si>
+  <si>
+    <t>checkClub</t>
+  </si>
+  <si>
+    <t>Adds or updates the club into the clubs table. If the item is there update using another method, if it does not exist then add using another method.</t>
+  </si>
+  <si>
+    <t>Adds or updates the accessory into the accessories table. If the item is there update using another method, if it does not exist then add using another method.</t>
+  </si>
+  <si>
+    <t>Adds or updates the clothing into the clothing table. If the item is there update using another method, if it does not exist then add using another method.</t>
+  </si>
+  <si>
+    <t>checkAccessory</t>
+  </si>
+  <si>
+    <t>checkClothing</t>
+  </si>
+  <si>
+    <t>convertDBNullToString</t>
+  </si>
+  <si>
+    <t>convertDBNullToDouble</t>
+  </si>
+  <si>
+    <t>Returns a 0 value double if the object is null.</t>
+  </si>
+  <si>
+    <t>Returns a blank string if the object is null.</t>
+  </si>
+  <si>
+    <t>getAccessory</t>
+  </si>
+  <si>
+    <t>Returns an accessory based on the sku that was input.</t>
+  </si>
+  <si>
+    <t>getClothing</t>
+  </si>
+  <si>
+    <t>Returns a clothing based on the sku that was input.</t>
+  </si>
+  <si>
+    <t>updateClub</t>
+  </si>
+  <si>
+    <t>Updates the info in the club table with the new info set as part of the club that was input.</t>
+  </si>
+  <si>
+    <t>Updates the info in the accessories table with the new info set as part of the accessory that was input.</t>
+  </si>
+  <si>
+    <t>Updates the info in the clothing table with the new info set as part of the clothing that was input.</t>
+  </si>
+  <si>
+    <t>updateAccessories</t>
+  </si>
+  <si>
+    <t>updateClothing</t>
+  </si>
+  <si>
+    <t>isTradein</t>
+  </si>
+  <si>
+    <t>Returns true or fsalse based on finding the sku in the club table and if the used was checked or not.</t>
+  </si>
+  <si>
+    <t>whatTypeIsItem</t>
+  </si>
+  <si>
+    <t>Returns the item type (club, accessory, clothing) value based on the sku that was input (duplicate method of something earlier in list)</t>
+  </si>
+  <si>
+    <t>getDescription</t>
+  </si>
+  <si>
+    <t>Returns the description of an item that is put together based on the item type that was input.</t>
+  </si>
+  <si>
+    <t>getInvoice</t>
+  </si>
+  <si>
+    <t>List&lt;Invoice&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of invoices that all have the same main invoice number based in the input</t>
+  </si>
+  <si>
+    <t>getInvoiceBySaleDate</t>
+  </si>
+  <si>
+    <t>DateTime, int</t>
+  </si>
+  <si>
+    <t>Returns a list of invoices based on the date and location passed in.</t>
+  </si>
+  <si>
+    <t>getSingleInvoice</t>
+  </si>
+  <si>
+    <t>Returns an Invoice that matches that invoice number and invoice sub number that was passed in.</t>
+  </si>
+  <si>
+    <t>multiTypeSearchInvoices</t>
+  </si>
+  <si>
+    <t>string, Nullable&lt;DateTime&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of invoices that match the searched criteria and the date that were input.</t>
+  </si>
+  <si>
+    <t>returningItems</t>
+  </si>
+  <si>
+    <t>Returns a list of cart items from the invoice item table that match the invoice number and invoice sub number that were passed in.</t>
+  </si>
+  <si>
+    <t>getInvoiceBetweenDates</t>
+  </si>
+  <si>
+    <t>DateTime, DateTime</t>
+  </si>
+  <si>
+    <t>Returns a list of Invoice class from the invoice table that fall between the dates that were input.</t>
+  </si>
+  <si>
+    <t>invoice_getCustID</t>
+  </si>
+  <si>
+    <t>invoice_getItems</t>
+  </si>
+  <si>
+    <t>Returns a list of cart items from the invoice item table that match the invoice number, invoice sub number and table that were passed in.</t>
+  </si>
+  <si>
+    <t>Returns the customer number based on the invoice number, invoice sub number and table that were passed in.</t>
+  </si>
+  <si>
+    <t>invoice_getCheckoutTotals</t>
+  </si>
+  <si>
+    <t>Returns a Checkout Manager class based on the invoice number, invoice sub number, and table that were passed in.</t>
+  </si>
+  <si>
+    <t>invoice_getMOP</t>
+  </si>
+  <si>
+    <t>List&lt;Checkout&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of checkout class items based on the invoice number, invoice sub number, and the table that were passed in.</t>
+  </si>
+  <si>
+    <t>invoice_getLocation</t>
+  </si>
+  <si>
+    <t>Returns the city name based on another procedure that uses the location ID based from the invoice number, invoice sub number, and table that were passed in.</t>
+  </si>
+  <si>
+    <t>deletedInvoice_getReason</t>
+  </si>
+  <si>
+    <t>Returns the text string reason for an invoice being deleted based on the invoice number and invoice sub number. Since deleting is no longer happening, this should no longer get used.</t>
+  </si>
+  <si>
+    <t>getTaxes</t>
+  </si>
+  <si>
+    <t>int, DateTime</t>
+  </si>
+  <si>
+    <t>List&lt;Tax&gt;</t>
+  </si>
+  <si>
+    <t>Returns a list of taxes based on the date and province ID that were passed in.</t>
+  </si>
+  <si>
+    <t>updateNewTaxRate</t>
+  </si>
+  <si>
+    <t>int, DateTime, int, double</t>
+  </si>
+  <si>
+    <t>Adds a new tax rate for a province based on a date. All are passed into the method.</t>
+  </si>
+  <si>
+    <t>Returns the total discounts applied in the cart as a total (duplicate method)</t>
+  </si>
+  <si>
+    <t>Returns the total trade in amount in the cart as a total(possible duplicate method)</t>
+  </si>
+  <si>
+    <t>Returns the total subtotal amount in the cart as a total(possible duplicate method)</t>
+  </si>
+  <si>
+    <t>returnRefundSubtotalAmount</t>
+  </si>
+  <si>
+    <t>Returns the total refund subtotal amount in the cart as a total(possible duplicate method)</t>
+  </si>
+  <si>
+    <t>Returns the total total amount in the cart as a total(possible duplicate method)</t>
+  </si>
+  <si>
+    <t>transferTradeInStart</t>
+  </si>
+  <si>
+    <t>transferTradeInDeleteOld</t>
+  </si>
+  <si>
+    <t>Loops through the clubs in the cart and finds any that are marked as a trade in. Then takes that club info and adds it into the club table then calls method to remove the old info from the temp trade in table.</t>
+  </si>
+  <si>
+    <t>This is the method that removes the trade in from the temp trade in table.</t>
+  </si>
+  <si>
+    <t>Creates a Sale class item (This class is not used at all)</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Creates a Tax class item</t>
+  </si>
+  <si>
+    <t>tbl_userinfo</t>
+  </si>
+  <si>
+    <t>Creates a tbl_userinfo class item</t>
+  </si>
+  <si>
+    <t>getuserinfologin</t>
+  </si>
+  <si>
+    <t>tbl_userinfomanager</t>
+  </si>
+  <si>
+    <t>Returns the employee ID as an interger based on the password used (duplicate method).</t>
   </si>
 </sst>
 </file>
@@ -309,8 +1233,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,21 +1564,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15D4FED-279A-43E8-9121-812C77A4D1D8}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,7 +1597,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -690,7 +1617,7 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -710,7 +1637,7 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -730,7 +1657,7 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -750,7 +1677,7 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -770,7 +1697,7 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -790,7 +1717,7 @@
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -810,7 +1737,7 @@
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -830,7 +1757,7 @@
       <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -838,7 +1765,7 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -846,7 +1773,7 @@
       <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -854,7 +1781,7 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -862,7 +1789,7 @@
       <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -870,7 +1797,7 @@
       <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -878,7 +1805,7 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -886,7 +1813,7 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -894,7 +1821,7 @@
       <c r="D17" t="s">
         <v>39</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -902,7 +1829,7 @@
       <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -910,7 +1837,7 @@
       <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -930,7 +1857,7 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -950,7 +1877,7 @@
       <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -970,7 +1897,7 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -990,7 +1917,7 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1010,7 +1937,7 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1030,7 +1957,7 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1050,7 +1977,7 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1070,7 +1997,7 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1090,7 +2017,7 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1110,7 +2037,7 @@
       <c r="E29">
         <v>110</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1118,7 +2045,7 @@
       <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1126,7 +2053,7 @@
       <c r="D31" t="s">
         <v>78</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1134,118 +2061,2743 @@
       <c r="D32" t="s">
         <v>80</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
       <c r="D33" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
       <c r="D34" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
       <c r="D35" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>18</v>
+      </c>
       <c r="D36" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
       <c r="D37" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
       <c r="D38" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
       <c r="D39" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
       <c r="D40" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
       <c r="D41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
       <c r="D42" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
       <c r="D43" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
       <c r="D44" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
       <c r="D45" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
       <c r="D46" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
       <c r="D47" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
       <c r="D48" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
       <c r="D49" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" t="s">
+        <v>118</v>
+      </c>
       <c r="D50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
       <c r="D51" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
       <c r="D52" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>10</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" t="s">
+        <v>60</v>
+      </c>
       <c r="D53" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
       <c r="D54" t="s">
         <v>82</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>60</v>
+      </c>
+      <c r="D57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" t="s">
+        <v>60</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>160</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>163</v>
+      </c>
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" t="s">
+        <v>82</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" t="s">
+        <v>82</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>170</v>
+      </c>
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" t="s">
+        <v>161</v>
+      </c>
+      <c r="C75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>176</v>
+      </c>
+      <c r="B76" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" t="s">
+        <v>60</v>
+      </c>
+      <c r="D76" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>181</v>
+      </c>
+      <c r="B78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" t="s">
+        <v>60</v>
+      </c>
+      <c r="D80" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C81" t="s">
+        <v>60</v>
+      </c>
+      <c r="D81" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" t="s">
+        <v>60</v>
+      </c>
+      <c r="D82" t="s">
+        <v>82</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>192</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>194</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>197</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" t="s">
+        <v>196</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>199</v>
+      </c>
+      <c r="B86" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" t="s">
+        <v>196</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" t="s">
+        <v>47</v>
+      </c>
+      <c r="D87" t="s">
+        <v>196</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" t="s">
+        <v>47</v>
+      </c>
+      <c r="C88" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" t="s">
+        <v>196</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>205</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" t="s">
+        <v>196</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" t="s">
+        <v>196</v>
+      </c>
+      <c r="E90">
+        <v>9</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>209</v>
+      </c>
+      <c r="B91" t="s">
+        <v>47</v>
+      </c>
+      <c r="C91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>196</v>
+      </c>
+      <c r="E91">
+        <v>8</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>211</v>
+      </c>
+      <c r="B92" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" t="s">
+        <v>18</v>
+      </c>
+      <c r="D92" t="s">
+        <v>196</v>
+      </c>
+      <c r="E92">
+        <v>3</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>213</v>
+      </c>
+      <c r="B93" t="s">
+        <v>47</v>
+      </c>
+      <c r="C93" t="s">
+        <v>194</v>
+      </c>
+      <c r="D93" t="s">
+        <v>196</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>47</v>
+      </c>
+      <c r="D94" t="s">
+        <v>196</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>219</v>
+      </c>
+      <c r="E95">
+        <v>120</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>221</v>
+      </c>
+      <c r="B96" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" t="s">
+        <v>219</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>225</v>
+      </c>
+      <c r="B97" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" t="s">
+        <v>227</v>
+      </c>
+      <c r="D97" t="s">
+        <v>224</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>228</v>
+      </c>
+      <c r="B98" t="s">
+        <v>226</v>
+      </c>
+      <c r="C98" t="s">
+        <v>227</v>
+      </c>
+      <c r="D98" t="s">
+        <v>224</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>229</v>
+      </c>
+      <c r="B99" t="s">
+        <v>226</v>
+      </c>
+      <c r="C99" t="s">
+        <v>52</v>
+      </c>
+      <c r="D99" t="s">
+        <v>224</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>233</v>
+      </c>
+      <c r="B100" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" t="s">
+        <v>224</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>235</v>
+      </c>
+      <c r="B101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C101" t="s">
+        <v>60</v>
+      </c>
+      <c r="D101" t="s">
+        <v>224</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>235</v>
+      </c>
+      <c r="B102" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" t="s">
+        <v>224</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>239</v>
+      </c>
+      <c r="C103" t="s">
+        <v>60</v>
+      </c>
+      <c r="D103" t="s">
+        <v>224</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>240</v>
+      </c>
+      <c r="C104" t="s">
+        <v>60</v>
+      </c>
+      <c r="D104" t="s">
+        <v>224</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>241</v>
+      </c>
+      <c r="C105" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" t="s">
+        <v>224</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>245</v>
+      </c>
+      <c r="C106" t="s">
+        <v>246</v>
+      </c>
+      <c r="D106" t="s">
+        <v>224</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" t="s">
+        <v>224</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>250</v>
+      </c>
+      <c r="C108" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" t="s">
+        <v>224</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" t="s">
+        <v>60</v>
+      </c>
+      <c r="D109" t="s">
+        <v>224</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>252</v>
+      </c>
+      <c r="C110" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" t="s">
+        <v>224</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>256</v>
+      </c>
+      <c r="C111" t="s">
+        <v>246</v>
+      </c>
+      <c r="D111" t="s">
+        <v>224</v>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>258</v>
+      </c>
+      <c r="C112" t="s">
+        <v>246</v>
+      </c>
+      <c r="D112" t="s">
+        <v>224</v>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" t="s">
+        <v>224</v>
+      </c>
+      <c r="E113">
+        <v>2</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" t="s">
+        <v>60</v>
+      </c>
+      <c r="D114" t="s">
+        <v>224</v>
+      </c>
+      <c r="E114">
+        <v>2</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>264</v>
+      </c>
+      <c r="C115" t="s">
+        <v>60</v>
+      </c>
+      <c r="D115" t="s">
+        <v>224</v>
+      </c>
+      <c r="E115">
+        <v>2</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>267</v>
+      </c>
+      <c r="C116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" t="s">
+        <v>224</v>
+      </c>
+      <c r="E116">
+        <v>2</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>268</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>270</v>
+      </c>
+      <c r="B118" t="s">
+        <v>47</v>
+      </c>
+      <c r="C118" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" t="s">
+        <v>269</v>
+      </c>
+      <c r="E118">
+        <v>2</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>272</v>
+      </c>
+      <c r="B119" t="s">
+        <v>18</v>
+      </c>
+      <c r="C119" t="s">
+        <v>41</v>
+      </c>
+      <c r="D119" t="s">
+        <v>269</v>
+      </c>
+      <c r="E119">
+        <v>10</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>275</v>
+      </c>
+      <c r="B120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C120" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" t="s">
+        <v>269</v>
+      </c>
+      <c r="E120">
+        <v>2</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>277</v>
+      </c>
+      <c r="B121" t="s">
+        <v>41</v>
+      </c>
+      <c r="C121" t="s">
+        <v>18</v>
+      </c>
+      <c r="D121" t="s">
+        <v>269</v>
+      </c>
+      <c r="E121">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>279</v>
+      </c>
+      <c r="B122" t="s">
+        <v>41</v>
+      </c>
+      <c r="C122" t="s">
+        <v>60</v>
+      </c>
+      <c r="D122" t="s">
+        <v>269</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>281</v>
+      </c>
+      <c r="B123" t="s">
+        <v>222</v>
+      </c>
+      <c r="C123" t="s">
+        <v>118</v>
+      </c>
+      <c r="D123" t="s">
+        <v>269</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>283</v>
+      </c>
+      <c r="B124" t="s">
+        <v>284</v>
+      </c>
+      <c r="C124" t="s">
+        <v>118</v>
+      </c>
+      <c r="D124" t="s">
+        <v>269</v>
+      </c>
+      <c r="E124">
+        <v>3</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>283</v>
+      </c>
+      <c r="B125" t="s">
+        <v>222</v>
+      </c>
+      <c r="C125" t="s">
+        <v>118</v>
+      </c>
+      <c r="D125" t="s">
+        <v>269</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>287</v>
+      </c>
+      <c r="B126" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" t="s">
+        <v>37</v>
+      </c>
+      <c r="D126" t="s">
+        <v>269</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>288</v>
+      </c>
+      <c r="B127" t="s">
+        <v>18</v>
+      </c>
+      <c r="C127" t="s">
+        <v>37</v>
+      </c>
+      <c r="D127" t="s">
+        <v>269</v>
+      </c>
+      <c r="E127">
+        <v>2</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>291</v>
+      </c>
+      <c r="B128" t="s">
+        <v>106</v>
+      </c>
+      <c r="C128" t="s">
+        <v>18</v>
+      </c>
+      <c r="D128" t="s">
+        <v>269</v>
+      </c>
+      <c r="E128">
+        <v>2</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>293</v>
+      </c>
+      <c r="B129" t="s">
+        <v>106</v>
+      </c>
+      <c r="C129" t="s">
+        <v>60</v>
+      </c>
+      <c r="D129" t="s">
+        <v>269</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>295</v>
+      </c>
+      <c r="B130" t="s">
+        <v>106</v>
+      </c>
+      <c r="C130" t="s">
+        <v>18</v>
+      </c>
+      <c r="D130" t="s">
+        <v>269</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" t="s">
+        <v>60</v>
+      </c>
+      <c r="D131" t="s">
+        <v>269</v>
+      </c>
+      <c r="E131">
+        <v>2</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>299</v>
+      </c>
+      <c r="B132" t="s">
+        <v>25</v>
+      </c>
+      <c r="C132" t="s">
+        <v>60</v>
+      </c>
+      <c r="D132" t="s">
+        <v>269</v>
+      </c>
+      <c r="E132">
+        <v>2</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>301</v>
+      </c>
+      <c r="B133" t="s">
+        <v>35</v>
+      </c>
+      <c r="C133" t="s">
+        <v>60</v>
+      </c>
+      <c r="D133" t="s">
+        <v>269</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>303</v>
+      </c>
+      <c r="B134" t="s">
+        <v>18</v>
+      </c>
+      <c r="C134" t="s">
+        <v>18</v>
+      </c>
+      <c r="D134" t="s">
+        <v>269</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>305</v>
+      </c>
+      <c r="B135" t="s">
+        <v>18</v>
+      </c>
+      <c r="C135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D135" t="s">
+        <v>269</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>306</v>
+      </c>
+      <c r="B136" t="s">
+        <v>18</v>
+      </c>
+      <c r="C136" t="s">
+        <v>68</v>
+      </c>
+      <c r="D136" t="s">
+        <v>269</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>307</v>
+      </c>
+      <c r="B137" t="s">
+        <v>18</v>
+      </c>
+      <c r="C137" t="s">
+        <v>68</v>
+      </c>
+      <c r="D137" t="s">
+        <v>269</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>311</v>
+      </c>
+      <c r="B138" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" t="s">
+        <v>60</v>
+      </c>
+      <c r="D138" t="s">
+        <v>269</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>315</v>
+      </c>
+      <c r="B139" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139" t="s">
+        <v>60</v>
+      </c>
+      <c r="D139" t="s">
+        <v>269</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>316</v>
+      </c>
+      <c r="B140" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" t="s">
+        <v>60</v>
+      </c>
+      <c r="D140" t="s">
+        <v>269</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>317</v>
+      </c>
+      <c r="B141" t="s">
+        <v>106</v>
+      </c>
+      <c r="C141" t="s">
+        <v>47</v>
+      </c>
+      <c r="D141" t="s">
+        <v>269</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>318</v>
+      </c>
+      <c r="B142" t="s">
+        <v>106</v>
+      </c>
+      <c r="C142" t="s">
+        <v>52</v>
+      </c>
+      <c r="D142" t="s">
+        <v>269</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>321</v>
+      </c>
+      <c r="B143" t="s">
+        <v>18</v>
+      </c>
+      <c r="C143" t="s">
+        <v>25</v>
+      </c>
+      <c r="D143" t="s">
+        <v>269</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>323</v>
+      </c>
+      <c r="B144" t="s">
+        <v>18</v>
+      </c>
+      <c r="C144" t="s">
+        <v>35</v>
+      </c>
+      <c r="D144" t="s">
+        <v>269</v>
+      </c>
+      <c r="E144">
+        <v>2</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>325</v>
+      </c>
+      <c r="B145" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145" t="s">
+        <v>60</v>
+      </c>
+      <c r="D145" t="s">
+        <v>269</v>
+      </c>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>329</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146" t="s">
+        <v>60</v>
+      </c>
+      <c r="D146" t="s">
+        <v>269</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>330</v>
+      </c>
+      <c r="B147" t="s">
+        <v>35</v>
+      </c>
+      <c r="C147" t="s">
+        <v>60</v>
+      </c>
+      <c r="D147" t="s">
+        <v>269</v>
+      </c>
+      <c r="E147">
+        <v>2</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>331</v>
+      </c>
+      <c r="B148" t="s">
+        <v>18</v>
+      </c>
+      <c r="C148" t="s">
+        <v>68</v>
+      </c>
+      <c r="D148" t="s">
+        <v>269</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>333</v>
+      </c>
+      <c r="B149" t="s">
+        <v>18</v>
+      </c>
+      <c r="C149" t="s">
+        <v>18</v>
+      </c>
+      <c r="D149" t="s">
+        <v>269</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>335</v>
+      </c>
+      <c r="B150" t="s">
+        <v>67</v>
+      </c>
+      <c r="C150" t="s">
+        <v>47</v>
+      </c>
+      <c r="D150" t="s">
+        <v>269</v>
+      </c>
+      <c r="E150">
+        <v>2</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>337</v>
+      </c>
+      <c r="B151" t="s">
+        <v>18</v>
+      </c>
+      <c r="C151" t="s">
+        <v>338</v>
+      </c>
+      <c r="D151" t="s">
+        <v>269</v>
+      </c>
+      <c r="E151">
+        <v>2</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>340</v>
+      </c>
+      <c r="B152" t="s">
+        <v>341</v>
+      </c>
+      <c r="C152" t="s">
+        <v>338</v>
+      </c>
+      <c r="D152" t="s">
+        <v>269</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>343</v>
+      </c>
+      <c r="B153" t="s">
+        <v>67</v>
+      </c>
+      <c r="C153" t="s">
+        <v>76</v>
+      </c>
+      <c r="D153" t="s">
+        <v>269</v>
+      </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>345</v>
+      </c>
+      <c r="B154" t="s">
+        <v>346</v>
+      </c>
+      <c r="C154" t="s">
+        <v>338</v>
+      </c>
+      <c r="D154" t="s">
+        <v>269</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>348</v>
+      </c>
+      <c r="B155" t="s">
+        <v>67</v>
+      </c>
+      <c r="C155" t="s">
+        <v>5</v>
+      </c>
+      <c r="D155" t="s">
+        <v>269</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>350</v>
+      </c>
+      <c r="B156" t="s">
+        <v>351</v>
+      </c>
+      <c r="C156" t="s">
+        <v>338</v>
+      </c>
+      <c r="D156" t="s">
+        <v>269</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>353</v>
+      </c>
+      <c r="B157" t="s">
+        <v>161</v>
+      </c>
+      <c r="C157" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" t="s">
+        <v>269</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>354</v>
+      </c>
+      <c r="B158" t="s">
+        <v>161</v>
+      </c>
+      <c r="C158" t="s">
+        <v>5</v>
+      </c>
+      <c r="D158" t="s">
+        <v>269</v>
+      </c>
+      <c r="E158">
+        <v>2</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>357</v>
+      </c>
+      <c r="B159" t="s">
+        <v>161</v>
+      </c>
+      <c r="C159" t="s">
+        <v>33</v>
+      </c>
+      <c r="D159" t="s">
+        <v>269</v>
+      </c>
+      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>359</v>
+      </c>
+      <c r="B160" t="s">
+        <v>161</v>
+      </c>
+      <c r="C160" t="s">
+        <v>360</v>
+      </c>
+      <c r="D160" t="s">
+        <v>269</v>
+      </c>
+      <c r="E160">
+        <v>2</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>362</v>
+      </c>
+      <c r="B161" t="s">
+        <v>161</v>
+      </c>
+      <c r="C161" t="s">
+        <v>47</v>
+      </c>
+      <c r="D161" t="s">
+        <v>269</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>364</v>
+      </c>
+      <c r="B162" t="s">
+        <v>67</v>
+      </c>
+      <c r="C162" t="s">
+        <v>47</v>
+      </c>
+      <c r="D162" t="s">
+        <v>269</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>366</v>
+      </c>
+      <c r="B163" t="s">
+        <v>367</v>
+      </c>
+      <c r="C163" t="s">
+        <v>368</v>
+      </c>
+      <c r="D163" t="s">
+        <v>269</v>
+      </c>
+      <c r="E163">
+        <v>5</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>370</v>
+      </c>
+      <c r="B164" t="s">
+        <v>371</v>
+      </c>
+      <c r="C164" t="s">
+        <v>60</v>
+      </c>
+      <c r="D164" t="s">
+        <v>269</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" t="s">
+        <v>52</v>
+      </c>
+      <c r="D165" t="s">
+        <v>269</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166" t="s">
+        <v>52</v>
+      </c>
+      <c r="D166" t="s">
+        <v>269</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167" t="s">
+        <v>5</v>
+      </c>
+      <c r="C167" t="s">
+        <v>52</v>
+      </c>
+      <c r="D167" t="s">
+        <v>269</v>
+      </c>
+      <c r="E167">
+        <v>6</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>376</v>
+      </c>
+      <c r="B168" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
+        <v>52</v>
+      </c>
+      <c r="D168" t="s">
+        <v>269</v>
+      </c>
+      <c r="E168">
+        <v>3</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>12</v>
+      </c>
+      <c r="B169" t="s">
+        <v>5</v>
+      </c>
+      <c r="C169" t="s">
+        <v>52</v>
+      </c>
+      <c r="D169" t="s">
+        <v>269</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>379</v>
+      </c>
+      <c r="B170" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170" t="s">
+        <v>60</v>
+      </c>
+      <c r="D170" t="s">
+        <v>269</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>380</v>
+      </c>
+      <c r="B171" t="s">
+        <v>18</v>
+      </c>
+      <c r="C171" t="s">
+        <v>60</v>
+      </c>
+      <c r="D171" t="s">
+        <v>269</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>384</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>386</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>388</v>
+      </c>
+      <c r="B174" t="s">
+        <v>18</v>
+      </c>
+      <c r="C174" t="s">
+        <v>18</v>
+      </c>
+      <c r="D174" t="s">
+        <v>389</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>